<commit_message>
making corrections with use case description in Portuguese
</commit_message>
<xml_diff>
--- a/Documentation/pt-BR/descricao/descricao_caso_de_uso.xlsx
+++ b/Documentation/pt-BR/descricao/descricao_caso_de_uso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="868" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="868" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Fazer Login" sheetId="8" r:id="rId1"/>
@@ -248,18 +248,6 @@
     </r>
   </si>
   <si>
-    <t>3. O usuário seleciona a categoria desejada e clica no botão de gerar nome.</t>
-  </si>
-  <si>
-    <t>4. O sistema apresenta o nome gerado.</t>
-  </si>
-  <si>
-    <t>4. O usuário clica no nome gerado.</t>
-  </si>
-  <si>
-    <t>5. O sistema copia o nome gerado para o teclado do celular do usuário.</t>
-  </si>
-  <si>
     <t>1. O usuário seleciona a opção de recuperação de senha.</t>
   </si>
   <si>
@@ -778,6 +766,18 @@
 IV. Senha
 V. Confirme a senha</t>
     </r>
+  </si>
+  <si>
+    <t>5. O usuário seleciona a categoria desejada e clica no botão de gerar nome.</t>
+  </si>
+  <si>
+    <t>7. O usuário clica no nome gerado.</t>
+  </si>
+  <si>
+    <t>8. O sistema copia o nome gerado para o teclado do celular do usuário.</t>
+  </si>
+  <si>
+    <t>6. O sistema apresenta o nome gerado.</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1213,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="6" spans="1:9" ht="96" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1381,7 +1381,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="2" spans="1:9" ht="33" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="6" spans="1:9" ht="106.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -1463,13 +1463,13 @@
     </row>
     <row r="7" spans="1:9" ht="35.25" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -1478,13 +1478,13 @@
     </row>
     <row r="8" spans="1:9" ht="51" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -1497,7 +1497,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="11" spans="1:9" ht="34.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1565,7 +1565,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1576,9 +1576,9 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="34.5" customHeight="1">
+    <row r="2" spans="1:9" ht="31.5" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1632,13 +1632,13 @@
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -1647,13 +1647,13 @@
     </row>
     <row r="7" spans="1:9" ht="33.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -1662,13 +1662,13 @@
     </row>
     <row r="8" spans="1:9" ht="51" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1810,7 +1810,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1924,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1999,13 +1999,13 @@
     </row>
     <row r="6" spans="1:9" ht="51" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -2014,13 +2014,13 @@
     </row>
     <row r="7" spans="1:9" ht="39.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -2033,7 +2033,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="10" spans="1:9" ht="32.25" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2092,7 +2092,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2166,13 +2166,13 @@
     </row>
     <row r="6" spans="1:9" ht="33" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -2181,13 +2181,13 @@
     </row>
     <row r="7" spans="1:9" ht="34.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -2196,13 +2196,13 @@
     </row>
     <row r="8" spans="1:9" ht="52.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="12" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -2211,13 +2211,13 @@
     </row>
     <row r="9" spans="1:9" ht="34.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="12" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -2284,7 +2284,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="2" spans="1:9" ht="33" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2351,13 +2351,13 @@
     </row>
     <row r="6" spans="1:9" ht="79.5" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -2366,13 +2366,13 @@
     </row>
     <row r="7" spans="1:9" ht="33.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -2381,13 +2381,13 @@
     </row>
     <row r="8" spans="1:9" ht="52.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -2400,7 +2400,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="11" spans="1:9" ht="34.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2468,7 +2468,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2481,7 +2481,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2535,13 +2535,13 @@
     </row>
     <row r="6" spans="1:9" ht="96" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -2550,13 +2550,13 @@
     </row>
     <row r="7" spans="1:9" ht="39" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -2569,7 +2569,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="10" spans="1:9" ht="33" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2636,7 +2636,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2703,13 +2703,13 @@
     </row>
     <row r="6" spans="1:9" ht="33.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -2722,7 +2722,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -2731,13 +2731,13 @@
     </row>
     <row r="8" spans="1:9" ht="108.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="10" spans="1:9" ht="36.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2803,7 +2803,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2814,9 +2814,9 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="21.75" customHeight="1">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2870,13 +2870,13 @@
     </row>
     <row r="6" spans="1:9" ht="110.25" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -2885,13 +2885,13 @@
     </row>
     <row r="7" spans="1:9" ht="35.25" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -2900,13 +2900,13 @@
     </row>
     <row r="8" spans="1:9" ht="64.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -2963,7 +2963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -2971,7 +2971,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2982,9 +2982,9 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3038,13 +3038,13 @@
     </row>
     <row r="6" spans="1:9" ht="107.25" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -3053,13 +3053,13 @@
     </row>
     <row r="7" spans="1:9" ht="56.25" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -3068,13 +3068,13 @@
     </row>
     <row r="8" spans="1:9" ht="58.5" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -3083,13 +3083,13 @@
     </row>
     <row r="9" spans="1:9" ht="58.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -3111,7 +3111,7 @@
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>

</xml_diff>